<commit_message>
support for error cells
</commit_message>
<xml_diff>
--- a/test/numbers.xlsx
+++ b/test/numbers.xlsx
@@ -1,86 +1,100 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noronha/.julia/v0.6/XLSX/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB265EAC-84A3-4D42-B24A-ADAA98263130}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{F22E95D4-159F-2747-9E88-4F92E855094B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="float" sheetId="1" r:id="rId1"/>
     <sheet name="int" sheetId="2" r:id="rId2"/>
+    <sheet name="error" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>errors</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="53">
-    <numFmt numFmtId="5" formatCode="&quot;R$&quot;#,##0;\-&quot;R$&quot;#,##0"/>
-    <numFmt numFmtId="6" formatCode="&quot;R$&quot;#,##0;[Red]\-&quot;R$&quot;#,##0"/>
-    <numFmt numFmtId="7" formatCode="&quot;R$&quot;#,##0.00;\-&quot;R$&quot;#,##0.00"/>
-    <numFmt numFmtId="8" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.0;[Red]0.0"/>
-    <numFmt numFmtId="166" formatCode="0.0_ ;\-0.0\ "/>
-    <numFmt numFmtId="167" formatCode="0.0_ ;[Red]\-0.0\ "/>
-    <numFmt numFmtId="168" formatCode="#,##0.0"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00;[Red]#,##0.00"/>
-    <numFmt numFmtId="170" formatCode="#,##0.0;[Red]#,##0.0"/>
-    <numFmt numFmtId="171" formatCode="#,##0.0_ ;\-#,##0.0\ "/>
-    <numFmt numFmtId="172" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
-    <numFmt numFmtId="173" formatCode="0.00;[Red]0.00"/>
-    <numFmt numFmtId="174" formatCode="0.00_ ;\-0.00\ "/>
-    <numFmt numFmtId="175" formatCode="0.00_ ;[Red]\-0.00\ "/>
-    <numFmt numFmtId="176" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-    <numFmt numFmtId="177" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-    <numFmt numFmtId="178" formatCode="0.000"/>
-    <numFmt numFmtId="179" formatCode="0.000;[Red]0.000"/>
-    <numFmt numFmtId="180" formatCode="0.000_ ;\-0.000\ "/>
-    <numFmt numFmtId="181" formatCode="0.000_ ;[Red]\-0.000\ "/>
-    <numFmt numFmtId="182" formatCode="#,##0.000"/>
-    <numFmt numFmtId="183" formatCode="#,##0.000;[Red]#,##0.000"/>
-    <numFmt numFmtId="184" formatCode="#,##0.000_ ;\-#,##0.000\ "/>
-    <numFmt numFmtId="185" formatCode="#,##0.000_ ;[Red]\-#,##0.000\ "/>
-    <numFmt numFmtId="186" formatCode="0.0000"/>
-    <numFmt numFmtId="187" formatCode="0.0000;[Red]0.0000"/>
-    <numFmt numFmtId="188" formatCode="0.0000_ ;\-0.0000\ "/>
-    <numFmt numFmtId="189" formatCode="0.0000_ ;[Red]\-0.0000\ "/>
-    <numFmt numFmtId="190" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="191" formatCode="#,##0.0000;[Red]#,##0.0000"/>
-    <numFmt numFmtId="192" formatCode="#,##0.0000_ ;\-#,##0.0000\ "/>
-    <numFmt numFmtId="193" formatCode="#,##0.0000_ ;[Red]\-#,##0.0000\ "/>
-    <numFmt numFmtId="195" formatCode="0.0E+00"/>
-    <numFmt numFmtId="196" formatCode="0.0%"/>
-    <numFmt numFmtId="197" formatCode="&quot;R$&quot;#,##0.0"/>
-    <numFmt numFmtId="198" formatCode="&quot;R$&quot;#,##0.0;[Red]&quot;R$&quot;#,##0.0"/>
-    <numFmt numFmtId="199" formatCode="&quot;R$&quot;#,##0.0;\-&quot;R$&quot;#,##0.0"/>
-    <numFmt numFmtId="200" formatCode="&quot;R$&quot;#,##0.0;[Red]\-&quot;R$&quot;#,##0.0"/>
-    <numFmt numFmtId="201" formatCode="&quot;R$&quot;#,##0.00"/>
-    <numFmt numFmtId="202" formatCode="&quot;R$&quot;#,##0.00;[Red]&quot;R$&quot;#,##0.00"/>
-    <numFmt numFmtId="203" formatCode="_-&quot;R$&quot;* #,##0.0_-;\-&quot;R$&quot;* #,##0.0_-;_-&quot;R$&quot;* &quot;-&quot;?_-;_-@_-"/>
-    <numFmt numFmtId="204" formatCode="0;[Red]0"/>
-    <numFmt numFmtId="205" formatCode="0_ ;\-0\ "/>
-    <numFmt numFmtId="206" formatCode="0_ ;[Red]\-0\ "/>
-    <numFmt numFmtId="207" formatCode="#,##0;[Red]#,##0"/>
-    <numFmt numFmtId="208" formatCode="#,##0_ ;\-#,##0\ "/>
-    <numFmt numFmtId="209" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    <numFmt numFmtId="210" formatCode="&quot;R$&quot;#,##0"/>
-    <numFmt numFmtId="211" formatCode="&quot;R$&quot;#,##0;[Red]&quot;R$&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;#,##0;\-&quot;R$&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="&quot;R$&quot;#,##0;[Red]\-&quot;R$&quot;#,##0"/>
+    <numFmt numFmtId="166" formatCode="&quot;R$&quot;#,##0.00;\-&quot;R$&quot;#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00"/>
+    <numFmt numFmtId="168" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="0.0;[Red]0.0"/>
+    <numFmt numFmtId="172" formatCode="0.0_ ;\-0.0\ "/>
+    <numFmt numFmtId="173" formatCode="0.0_ ;[Red]\-0.0\ "/>
+    <numFmt numFmtId="174" formatCode="#,##0.0"/>
+    <numFmt numFmtId="175" formatCode="#,##0.00;[Red]#,##0.00"/>
+    <numFmt numFmtId="176" formatCode="#,##0.0;[Red]#,##0.0"/>
+    <numFmt numFmtId="177" formatCode="#,##0.0_ ;\-#,##0.0\ "/>
+    <numFmt numFmtId="178" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
+    <numFmt numFmtId="179" formatCode="0.00;[Red]0.00"/>
+    <numFmt numFmtId="180" formatCode="0.00_ ;\-0.00\ "/>
+    <numFmt numFmtId="181" formatCode="0.00_ ;[Red]\-0.00\ "/>
+    <numFmt numFmtId="182" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+    <numFmt numFmtId="183" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+    <numFmt numFmtId="184" formatCode="0.000"/>
+    <numFmt numFmtId="185" formatCode="0.000;[Red]0.000"/>
+    <numFmt numFmtId="186" formatCode="0.000_ ;\-0.000\ "/>
+    <numFmt numFmtId="187" formatCode="0.000_ ;[Red]\-0.000\ "/>
+    <numFmt numFmtId="188" formatCode="#,##0.000"/>
+    <numFmt numFmtId="189" formatCode="#,##0.000;[Red]#,##0.000"/>
+    <numFmt numFmtId="190" formatCode="#,##0.000_ ;\-#,##0.000\ "/>
+    <numFmt numFmtId="191" formatCode="#,##0.000_ ;[Red]\-#,##0.000\ "/>
+    <numFmt numFmtId="192" formatCode="0.0000"/>
+    <numFmt numFmtId="193" formatCode="0.0000;[Red]0.0000"/>
+    <numFmt numFmtId="194" formatCode="0.0000_ ;\-0.0000\ "/>
+    <numFmt numFmtId="195" formatCode="0.0000_ ;[Red]\-0.0000\ "/>
+    <numFmt numFmtId="196" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="197" formatCode="#,##0.0000;[Red]#,##0.0000"/>
+    <numFmt numFmtId="198" formatCode="#,##0.0000_ ;\-#,##0.0000\ "/>
+    <numFmt numFmtId="199" formatCode="#,##0.0000_ ;[Red]\-#,##0.0000\ "/>
+    <numFmt numFmtId="200" formatCode="0.0E+00"/>
+    <numFmt numFmtId="201" formatCode="0.0%"/>
+    <numFmt numFmtId="202" formatCode="&quot;R$&quot;#,##0.0"/>
+    <numFmt numFmtId="203" formatCode="&quot;R$&quot;#,##0.0;[Red]&quot;R$&quot;#,##0.0"/>
+    <numFmt numFmtId="204" formatCode="&quot;R$&quot;#,##0.0;\-&quot;R$&quot;#,##0.0"/>
+    <numFmt numFmtId="205" formatCode="&quot;R$&quot;#,##0.0;[Red]\-&quot;R$&quot;#,##0.0"/>
+    <numFmt numFmtId="206" formatCode="&quot;R$&quot;#,##0.00"/>
+    <numFmt numFmtId="207" formatCode="&quot;R$&quot;#,##0.00;[Red]&quot;R$&quot;#,##0.00"/>
+    <numFmt numFmtId="208" formatCode="_-&quot;R$&quot;* #,##0.0_-;\-&quot;R$&quot;* #,##0.0_-;_-&quot;R$&quot;* &quot;-&quot;?_-;_-@_-"/>
+    <numFmt numFmtId="209" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="210" formatCode="0_ ;\-0\ "/>
+    <numFmt numFmtId="211" formatCode="0_ ;[Red]\-0\ "/>
+    <numFmt numFmtId="212" formatCode="#,##0;[Red]#,##0"/>
+    <numFmt numFmtId="213" formatCode="#,##0_ ;\-#,##0\ "/>
+    <numFmt numFmtId="214" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="215" formatCode="&quot;R$&quot;#,##0"/>
+    <numFmt numFmtId="216" formatCode="&quot;R$&quot;#,##0;[Red]&quot;R$&quot;#,##0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -113,26 +127,20 @@
   </cellStyleXfs>
   <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -145,34 +153,40 @@
     <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="192" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="193" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="194" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="195" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="196" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="197" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="198" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="199" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="200" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="201" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="202" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="203" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="204" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="205" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="206" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="207" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="208" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="209" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="210" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="211" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="212" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="213" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="214" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="215" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="216" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,7 +500,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10769357-B609-C84D-89A3-43A22825BB63}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -717,7 +731,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9441E3-FD1A-9C4E-ABC7-E027EDEF8576}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -804,4 +818,42 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="e">
+        <f>A1+1</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="e">
+        <f>undefined_function</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="e">
+        <f>10/0</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>